<commit_message>
Added user friendly names that match our guidelines.
</commit_message>
<xml_diff>
--- a/examples/spreadsheets/current/filled/filled_example_SS2.xlsx
+++ b/examples/spreadsheets/current/filled/filled_example_SS2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10309"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/Desktop/spreadsheet_test/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/enrique/HumanCellAtlas/metadata-schema/examples/spreadsheets/current/filled/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEAFEC4E-C7DB-344B-9A96-E3862602C208}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC9B2224-60E0-3E47-A632-A3B8E475C406}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="51200" windowHeight="27320" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20160" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Project" sheetId="1" r:id="rId1"/>
@@ -353,7 +353,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1129" uniqueCount="617">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1126" uniqueCount="615">
   <si>
     <t>AUTHORS (Required)</t>
   </si>
@@ -844,9 +844,6 @@
     <t>Joshua,Z,Levin</t>
   </si>
   <si>
-    <t>jlevin@broadinstitute.org</t>
-  </si>
-  <si>
     <t>yes</t>
   </si>
   <si>
@@ -886,15 +883,9 @@
     <t>William,G,Sullivan</t>
   </si>
   <si>
-    <t>wisulliv@ucsc.edu</t>
-  </si>
-  <si>
     <t>Parisa,,Nejad</t>
   </si>
   <si>
-    <t>pnejad@ucsc.edu</t>
-  </si>
-  <si>
     <t>0000-0002-3163-0115</t>
   </si>
   <si>
@@ -2104,30 +2095,9 @@
     <t>Ding J||Adiconis X||Simmons SK||Kowalczyk MS||Hession CC||Marjanovic ND||Hughes TK||MH Wadsworth MH||Burks T||Nguyen LT||Kwon JY||Barak B||Ge W||Kedaigle AJ||Carroll S||Li S||Hacohen N||Rozenblatt-Rosen O||Shalek AK||Villani C||Regev A||Levin JZ</t>
   </si>
   <si>
-    <t>SPECIMEN ID (Required)</t>
-  </si>
-  <si>
-    <t>SPECIMEN NAME</t>
-  </si>
-  <si>
-    <t>SPECIMEN DESCRIPTION</t>
-  </si>
-  <si>
     <t>collection_protocol</t>
   </si>
   <si>
-    <t>INPUT SPECIMEN ID (Required)</t>
-  </si>
-  <si>
-    <t>PROTOCOL NAME</t>
-  </si>
-  <si>
-    <t>PROTOCOL ID</t>
-  </si>
-  <si>
-    <t>PROTOCOL DESCRIPTION</t>
-  </si>
-  <si>
     <t>For example: 10.1101/193219</t>
   </si>
   <si>
@@ -2185,9 +2155,6 @@
     <t>data:3494</t>
   </si>
   <si>
-    <t>PROTOCOL ID (Required)</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 100 µm nozzle to sort single cells into 96-well plates containing 5 µl TCL buffer (Qiagen) with 1% beta-mercaptoethanol for Smart-seq2 and 384-well plates containing 0.6 µl 1% NP40 (Thermo Fisher Scientific) for CEL-Seq2</t>
   </si>
   <si>
@@ -2204,6 +2171,33 @@
   </si>
   <si>
     <t>process.process_core.process_id</t>
+  </si>
+  <si>
+    <t>SPECIMEN FROM ORGANISM ID (Required)</t>
+  </si>
+  <si>
+    <t>SPECIMEN FROM ORGANISM NAME</t>
+  </si>
+  <si>
+    <t>SPECIMEN FROM ORGANISM DESCRIPTION</t>
+  </si>
+  <si>
+    <t>INPUT SPECIMEN FROM ORGANISM ID (Required)</t>
+  </si>
+  <si>
+    <t>ENRICHMENT PROTOCOL ID</t>
+  </si>
+  <si>
+    <t>ENRICHMENT PROTOCOL NAME</t>
+  </si>
+  <si>
+    <t>ENRICHMENT PROTOCOL DESCRIPTION</t>
+  </si>
+  <si>
+    <t>DISSOCIATION PROTOCOL NAME</t>
+  </si>
+  <si>
+    <t>DISSOCIATION PROTOCOL DESCRIPTION</t>
   </si>
 </sst>
 </file>
@@ -2647,7 +2641,7 @@
   <dimension ref="A1:I999"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I4" sqref="I4"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -3805,8 +3799,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:P991"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -3831,75 +3825,75 @@
   <sheetData>
     <row r="1" spans="1:16" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>366</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>342</v>
+      </c>
+      <c r="F1" s="12" t="s">
+        <v>375</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>367</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>368</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>369</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>587</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>345</v>
-      </c>
-      <c r="F1" s="12" t="s">
-        <v>378</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>184</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>187</v>
-      </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>370</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>372</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>373</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>375</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>376</v>
-      </c>
       <c r="O1" s="1" t="s">
-        <v>614</v>
+        <v>603</v>
       </c>
     </row>
     <row r="2" spans="1:16" ht="68">
       <c r="A2" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="G2" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>201</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>200</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>250</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>203</v>
-      </c>
       <c r="H2" s="2" t="s">
-        <v>388</v>
+        <v>385</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>65</v>
@@ -3908,7 +3902,7 @@
         <v>66</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>389</v>
+        <v>386</v>
       </c>
       <c r="L2" s="2" t="s">
         <v>65</v>
@@ -3917,10 +3911,10 @@
         <v>66</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>390</v>
+        <v>387</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>612</v>
+        <v>601</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="102">
@@ -3929,84 +3923,84 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="K3" s="2" t="s">
+        <v>393</v>
+      </c>
+      <c r="L3" s="2" t="s">
+        <v>394</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="N3" s="2" t="s">
         <v>396</v>
       </c>
-      <c r="L3" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="M3" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="N3" s="2" t="s">
-        <v>399</v>
-      </c>
       <c r="O3" s="2" t="s">
-        <v>613</v>
+        <v>602</v>
       </c>
     </row>
     <row r="4" spans="1:16" hidden="1">
       <c r="A4" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>411</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>400</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>401</v>
       </c>
-      <c r="C4" s="3" t="s">
-        <v>402</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>296</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>349</v>
-      </c>
-      <c r="F4" s="5" t="s">
-        <v>414</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>403</v>
       </c>
-      <c r="H4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>404</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="K4" s="3" t="s">
+        <v>405</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>406</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>407</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>408</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>409</v>
-      </c>
-      <c r="M4" s="3" t="s">
-        <v>410</v>
-      </c>
-      <c r="N4" s="3" t="s">
-        <v>411</v>
-      </c>
-      <c r="O4" s="3" t="s">
-        <v>412</v>
       </c>
     </row>
     <row r="5" spans="1:16" ht="30" customHeight="1">
@@ -4030,96 +4024,96 @@
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="3" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>325</v>
+        <v>322</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="G6" s="3">
         <v>9606</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="N6" s="5">
         <v>311</v>
       </c>
       <c r="O6" s="3" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="7" spans="1:16" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>461</v>
+        <v>458</v>
       </c>
       <c r="G7" s="3">
         <v>9606</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>450</v>
+        <v>447</v>
       </c>
       <c r="M7" s="3" t="s">
-        <v>449</v>
+        <v>446</v>
       </c>
       <c r="N7" s="5">
         <v>273</v>
       </c>
       <c r="O7" s="3" t="s">
-        <v>456</v>
+        <v>453</v>
       </c>
     </row>
     <row r="8" spans="1:16" ht="15.75" customHeight="1">
@@ -5325,69 +5319,69 @@
   <sheetData>
     <row r="1" spans="1:14" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>412</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>413</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>415</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>416</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>416</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>419</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
+        <v>420</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>421</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>422</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>423</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>424</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>425</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>426</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>429</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>430</v>
+        <v>427</v>
       </c>
     </row>
     <row r="2" spans="1:14" ht="92" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>253</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>65</v>
@@ -5396,13 +5390,13 @@
         <v>66</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>438</v>
+        <v>435</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>439</v>
+        <v>436</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="M2" s="2" t="s">
         <v>65</v>
@@ -5413,86 +5407,86 @@
     </row>
     <row r="3" spans="1:14" ht="92" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>451</v>
+        <v>448</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>447</v>
+        <v>444</v>
       </c>
       <c r="J3" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="K3" s="2" t="s">
+        <v>454</v>
+      </c>
+      <c r="L3" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="K3" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="L3" s="2" t="s">
-        <v>458</v>
-      </c>
       <c r="M3" s="2" t="s">
-        <v>459</v>
+        <v>456</v>
       </c>
       <c r="N3" s="2" t="s">
-        <v>458</v>
+        <v>455</v>
       </c>
     </row>
     <row r="4" spans="1:14" hidden="1">
       <c r="A4" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>461</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>462</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>463</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>464</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>465</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>466</v>
-      </c>
-      <c r="F4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>467</v>
       </c>
-      <c r="G4" s="3" t="s">
-        <v>468</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>470</v>
-      </c>
       <c r="I4" s="3" t="s">
-        <v>472</v>
+        <v>469</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>474</v>
+        <v>471</v>
       </c>
       <c r="K4" s="3" t="s">
-        <v>476</v>
+        <v>473</v>
       </c>
       <c r="L4" s="3" t="s">
-        <v>478</v>
+        <v>475</v>
       </c>
       <c r="M4" s="3" t="s">
-        <v>480</v>
+        <v>477</v>
       </c>
       <c r="N4" s="3" t="s">
-        <v>482</v>
+        <v>479</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="30" customHeight="1">
@@ -5515,29 +5509,29 @@
     </row>
     <row r="6" spans="1:14">
       <c r="A6" s="3" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>495</v>
+        <v>492</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>494</v>
+        <v>491</v>
       </c>
       <c r="J6" s="3"/>
       <c r="K6" s="3" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>496</v>
+        <v>493</v>
       </c>
       <c r="M6" s="3" t="s">
-        <v>497</v>
+        <v>494</v>
       </c>
       <c r="N6" s="3" t="s">
-        <v>498</v>
+        <v>495</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="15" customHeight="1">
@@ -6537,7 +6531,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A1:U1140"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
@@ -6568,81 +6562,81 @@
   <sheetData>
     <row r="1" spans="1:21" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>369</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>371</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>372</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>374</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>376</v>
+      </c>
+      <c r="F1" s="1" t="s">
         <v>377</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="G1" s="1" t="s">
+        <v>378</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>379</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>380</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>381</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>382</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>383</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>384</v>
       </c>
-      <c r="K1" s="1" t="s">
-        <v>385</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>386</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>387</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>598</v>
+        <v>588</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>599</v>
+        <v>589</v>
       </c>
       <c r="P1" s="1" t="s">
-        <v>600</v>
+        <v>590</v>
       </c>
       <c r="Q1" s="1" t="s">
+        <v>388</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>389</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>390</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>391</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>392</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>393</v>
-      </c>
-      <c r="T1" s="1" t="s">
-        <v>394</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>395</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="134" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>253</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>405</v>
+        <v>402</v>
       </c>
       <c r="E2" s="2" t="s">
         <v>65</v>
@@ -6651,10 +6645,10 @@
         <v>66</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>417</v>
+        <v>414</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>65</v>
@@ -6663,25 +6657,25 @@
         <v>66</v>
       </c>
       <c r="K2" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="L2" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="M2" s="2" t="s">
         <v>418</v>
       </c>
-      <c r="L2" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="M2" s="2" t="s">
-        <v>421</v>
-      </c>
       <c r="N2" s="2" t="s">
-        <v>601</v>
+        <v>591</v>
       </c>
       <c r="O2" s="2" t="s">
-        <v>603</v>
+        <v>593</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>605</v>
+        <v>595</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>65</v>
@@ -6690,136 +6684,136 @@
         <v>66</v>
       </c>
       <c r="T2" s="2" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="U2" s="2" t="s">
-        <v>428</v>
+        <v>425</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="93" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>431</v>
+        <v>428</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>429</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>430</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>432</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="H3" s="2" t="s">
         <v>433</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>436</v>
-      </c>
       <c r="I3" s="2" t="s">
+        <v>434</v>
+      </c>
+      <c r="J3" s="2" t="s">
+        <v>433</v>
+      </c>
+      <c r="K3" s="2" t="s">
         <v>437</v>
       </c>
-      <c r="J3" s="2" t="s">
-        <v>436</v>
-      </c>
-      <c r="K3" s="2" t="s">
-        <v>440</v>
-      </c>
       <c r="L3" s="2" t="s">
+        <v>438</v>
+      </c>
+      <c r="M3" s="2" t="s">
+        <v>439</v>
+      </c>
+      <c r="N3" s="2" t="s">
+        <v>592</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>594</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>596</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>441</v>
       </c>
-      <c r="M3" s="2" t="s">
+      <c r="R3" s="2" t="s">
         <v>442</v>
       </c>
-      <c r="N3" s="2" t="s">
-        <v>602</v>
-      </c>
-      <c r="O3" s="2" t="s">
-        <v>604</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>606</v>
-      </c>
-      <c r="Q3" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="R3" s="2" t="s">
+      <c r="S3" s="2" t="s">
+        <v>441</v>
+      </c>
+      <c r="T3" s="2" t="s">
+        <v>443</v>
+      </c>
+      <c r="U3" s="2" t="s">
         <v>445</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>444</v>
-      </c>
-      <c r="T3" s="2" t="s">
-        <v>446</v>
-      </c>
-      <c r="U3" s="2" t="s">
-        <v>448</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="19" hidden="1" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>453</v>
+        <v>450</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>454</v>
+        <v>451</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>460</v>
+        <v>457</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>469</v>
+        <v>466</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>471</v>
+        <v>468</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>473</v>
+        <v>470</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>475</v>
+        <v>472</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>477</v>
+        <v>474</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>479</v>
+        <v>476</v>
       </c>
       <c r="K4" s="3" t="s">
+        <v>478</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>480</v>
+      </c>
+      <c r="M4" s="3" t="s">
         <v>481</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="N4" s="3" t="s">
+        <v>482</v>
+      </c>
+      <c r="O4" s="3" t="s">
         <v>483</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>484</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>485</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>486</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>487</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>488</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>489</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>490</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>491</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>492</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="30" customHeight="1">
@@ -6849,57 +6843,57 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" s="3" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>597</v>
+        <v>587</v>
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="3"/>
       <c r="G6" s="3" t="s">
-        <v>499</v>
+        <v>496</v>
       </c>
       <c r="H6" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>502</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>501</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="L6" s="3" t="s">
+        <v>497</v>
+      </c>
+      <c r="M6" s="3" t="s">
+        <v>503</v>
+      </c>
+      <c r="N6" s="3" t="s">
         <v>504</v>
-      </c>
-      <c r="I6" s="3" t="s">
-        <v>505</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>504</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>496</v>
-      </c>
-      <c r="L6" s="3" t="s">
-        <v>500</v>
-      </c>
-      <c r="M6" s="3" t="s">
-        <v>506</v>
-      </c>
-      <c r="N6" s="3" t="s">
-        <v>507</v>
       </c>
       <c r="O6" s="3">
         <v>4456739</v>
       </c>
       <c r="P6" s="3" t="s">
-        <v>607</v>
+        <v>597</v>
       </c>
       <c r="Q6" s="3" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>502</v>
+        <v>499</v>
       </c>
       <c r="S6" s="3" t="s">
-        <v>501</v>
+        <v>498</v>
       </c>
       <c r="T6" s="3"/>
       <c r="U6" s="3"/>
@@ -10356,54 +10350,54 @@
   <sheetData>
     <row r="1" spans="1:15" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>368</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>410</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="G1" s="1" t="s">
         <v>508</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>516</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>371</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>413</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>509</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>510</v>
-      </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>511</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>513</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>512</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>515</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>514</v>
       </c>
     </row>
     <row r="2" spans="1:15" ht="111" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>517</v>
+        <v>514</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>518</v>
+        <v>515</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>65</v>
@@ -10412,85 +10406,85 @@
         <v>66</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>520</v>
+        <v>517</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>519</v>
+        <v>516</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>521</v>
+        <v>518</v>
       </c>
       <c r="K2" s="2"/>
     </row>
     <row r="3" spans="1:15" ht="111" customHeight="1">
       <c r="A3" s="2" t="s">
-        <v>522</v>
+        <v>519</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>520</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>522</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>521</v>
+      </c>
+      <c r="H3" s="2" t="s">
         <v>523</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>525</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="H3" s="2" t="s">
-        <v>526</v>
       </c>
       <c r="I3" s="2">
         <v>1</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>528</v>
+        <v>525</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>527</v>
+        <v>524</v>
       </c>
     </row>
     <row r="4" spans="1:15">
       <c r="A4" s="3" t="s">
+        <v>526</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>449</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>527</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>528</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>529</v>
       </c>
-      <c r="B4" s="3" t="s">
-        <v>400</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>452</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>462</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="H4" s="3" t="s">
+        <v>531</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>530</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>531</v>
-      </c>
-      <c r="G4" s="3" t="s">
+      <c r="J4" s="3" t="s">
+        <v>533</v>
+      </c>
+      <c r="K4" s="3" t="s">
         <v>532</v>
       </c>
-      <c r="H4" s="3" t="s">
-        <v>534</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>533</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>536</v>
-      </c>
-      <c r="K4" s="3" t="s">
-        <v>535</v>
-      </c>
       <c r="L4" s="30" t="s">
-        <v>616</v>
+        <v>605</v>
       </c>
     </row>
     <row r="5" spans="1:15" ht="30" customHeight="1">
@@ -10510,28 +10504,28 @@
     </row>
     <row r="6" spans="1:15" ht="15.75" customHeight="1">
       <c r="A6" s="3" t="s">
-        <v>564</v>
+        <v>561</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>609</v>
+        <v>599</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="I6" s="3">
         <v>1</v>
@@ -10540,10 +10534,10 @@
         <v>50</v>
       </c>
       <c r="K6" s="3" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="L6" s="3" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="M6" s="13"/>
       <c r="N6" s="13"/>
@@ -10551,28 +10545,28 @@
     </row>
     <row r="7" spans="1:15" ht="15.75" customHeight="1">
       <c r="A7" s="3" t="s">
-        <v>566</v>
+        <v>563</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>609</v>
+        <v>599</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="I7" s="3">
         <v>1</v>
@@ -10581,10 +10575,10 @@
         <v>50</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="L7" s="3" t="s">
-        <v>565</v>
+        <v>562</v>
       </c>
       <c r="M7" s="13"/>
       <c r="N7" s="13"/>
@@ -10592,28 +10586,28 @@
     </row>
     <row r="8" spans="1:15" ht="15.75" customHeight="1">
       <c r="A8" s="3" t="s">
-        <v>567</v>
+        <v>564</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>609</v>
+        <v>599</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="I8" s="3">
         <v>1</v>
@@ -10622,10 +10616,10 @@
         <v>50</v>
       </c>
       <c r="K8" s="3" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="L8" s="3" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="M8" s="13"/>
       <c r="N8" s="13"/>
@@ -10633,28 +10627,28 @@
     </row>
     <row r="9" spans="1:15" ht="15.75" customHeight="1">
       <c r="A9" s="3" t="s">
-        <v>569</v>
+        <v>566</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>609</v>
+        <v>599</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="I9" s="3">
         <v>1</v>
@@ -10663,10 +10657,10 @@
         <v>50</v>
       </c>
       <c r="K9" s="3" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="L9" s="3" t="s">
-        <v>568</v>
+        <v>565</v>
       </c>
       <c r="M9" s="13"/>
       <c r="N9" s="13"/>
@@ -10674,28 +10668,28 @@
     </row>
     <row r="10" spans="1:15" ht="15.75" customHeight="1">
       <c r="A10" s="3" t="s">
-        <v>570</v>
+        <v>567</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>609</v>
+        <v>599</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="I10" s="3">
         <v>1</v>
@@ -10704,10 +10698,10 @@
         <v>50</v>
       </c>
       <c r="K10" s="3" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="L10" s="3" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="M10" s="13"/>
       <c r="N10" s="13"/>
@@ -10715,28 +10709,28 @@
     </row>
     <row r="11" spans="1:15" ht="15.75" customHeight="1">
       <c r="A11" s="3" t="s">
-        <v>572</v>
+        <v>569</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>443</v>
+        <v>440</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>609</v>
+        <v>599</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="I11" s="3">
         <v>1</v>
@@ -10745,10 +10739,10 @@
         <v>50</v>
       </c>
       <c r="K11" s="3" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="L11" s="3" t="s">
-        <v>571</v>
+        <v>568</v>
       </c>
       <c r="M11" s="13"/>
       <c r="N11" s="13"/>
@@ -10756,28 +10750,28 @@
     </row>
     <row r="12" spans="1:15" ht="15.75" customHeight="1">
       <c r="A12" s="3" t="s">
-        <v>573</v>
+        <v>570</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>609</v>
+        <v>599</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="I12" s="3">
         <v>1</v>
@@ -10786,10 +10780,10 @@
         <v>50</v>
       </c>
       <c r="K12" s="3" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="L12" s="3" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="M12" s="13"/>
       <c r="N12" s="13"/>
@@ -10797,28 +10791,28 @@
     </row>
     <row r="13" spans="1:15" ht="15.75" customHeight="1">
       <c r="A13" s="3" t="s">
-        <v>575</v>
+        <v>572</v>
       </c>
       <c r="B13" s="3" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C13" s="3" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D13" s="3" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
       <c r="E13" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F13" s="3" t="s">
-        <v>609</v>
+        <v>599</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="H13" s="3" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="I13" s="3">
         <v>1</v>
@@ -10827,10 +10821,10 @@
         <v>50</v>
       </c>
       <c r="K13" s="3" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="L13" s="3" t="s">
-        <v>574</v>
+        <v>571</v>
       </c>
       <c r="M13" s="13"/>
       <c r="N13" s="13"/>
@@ -10838,28 +10832,28 @@
     </row>
     <row r="14" spans="1:15" ht="15.75" customHeight="1">
       <c r="A14" s="3" t="s">
-        <v>576</v>
+        <v>573</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C14" s="3" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D14" s="3" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
       <c r="E14" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F14" s="3" t="s">
-        <v>609</v>
+        <v>599</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="H14" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="I14" s="3">
         <v>1</v>
@@ -10868,10 +10862,10 @@
         <v>50</v>
       </c>
       <c r="K14" s="3" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="L14" s="3" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="M14" s="13"/>
       <c r="N14" s="13"/>
@@ -10879,28 +10873,28 @@
     </row>
     <row r="15" spans="1:15" ht="15.75" customHeight="1">
       <c r="A15" s="3" t="s">
-        <v>578</v>
+        <v>575</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
       <c r="E15" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F15" s="3" t="s">
-        <v>609</v>
+        <v>599</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="H15" s="3" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="I15" s="3">
         <v>1</v>
@@ -10909,10 +10903,10 @@
         <v>50</v>
       </c>
       <c r="K15" s="3" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="L15" s="3" t="s">
-        <v>577</v>
+        <v>574</v>
       </c>
       <c r="M15" s="13"/>
       <c r="N15" s="13"/>
@@ -10920,28 +10914,28 @@
     </row>
     <row r="16" spans="1:15" ht="15.75" customHeight="1">
       <c r="A16" s="3" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D16" s="3" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F16" s="3" t="s">
-        <v>609</v>
+        <v>599</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="H16" s="3" t="s">
-        <v>542</v>
+        <v>539</v>
       </c>
       <c r="I16" s="3">
         <v>1</v>
@@ -10950,10 +10944,10 @@
         <v>50</v>
       </c>
       <c r="K16" s="3" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="L16" s="3" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="M16" s="13"/>
       <c r="N16" s="13"/>
@@ -10961,28 +10955,28 @@
     </row>
     <row r="17" spans="1:15" ht="15.75" customHeight="1">
       <c r="A17" s="3" t="s">
-        <v>581</v>
+        <v>578</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>503</v>
+        <v>500</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>504</v>
+        <v>501</v>
       </c>
       <c r="D17" s="3" t="s">
-        <v>615</v>
+        <v>604</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>538</v>
+        <v>535</v>
       </c>
       <c r="F17" s="3" t="s">
-        <v>609</v>
+        <v>599</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>608</v>
+        <v>598</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>544</v>
+        <v>541</v>
       </c>
       <c r="I17" s="3">
         <v>1</v>
@@ -10991,10 +10985,10 @@
         <v>50</v>
       </c>
       <c r="K17" s="3" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="L17" s="3" t="s">
-        <v>580</v>
+        <v>577</v>
       </c>
       <c r="M17" s="13"/>
       <c r="N17" s="13"/>
@@ -11012,7 +11006,7 @@
   <dimension ref="A1:L1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F12" sqref="F12"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -11839,9 +11833,7 @@
       <c r="A27" s="3" t="s">
         <v>162</v>
       </c>
-      <c r="B27" s="3" t="s">
-        <v>163</v>
-      </c>
+      <c r="B27" s="3"/>
       <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
         <v>109</v>
@@ -11856,30 +11848,30 @@
         <v>112</v>
       </c>
       <c r="H27" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="I27" s="3" t="s">
         <v>164</v>
       </c>
-      <c r="I27" s="3" t="s">
+      <c r="J27" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="J27" s="8" t="s">
+      <c r="K27" s="8" t="s">
+        <v>164</v>
+      </c>
+      <c r="L27" s="3" t="s">
         <v>166</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>165</v>
-      </c>
-      <c r="L27" s="3" t="s">
-        <v>167</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1">
       <c r="A28" s="3" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="D28" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E28" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="G28" s="3" t="s">
         <v>112</v>
@@ -11888,27 +11880,25 @@
         <v>113</v>
       </c>
       <c r="I28" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="J28" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="J28" s="8" t="s">
+      <c r="K28" s="8" t="s">
         <v>174</v>
-      </c>
-      <c r="K28" s="8" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1">
       <c r="A29" s="3" t="s">
-        <v>176</v>
-      </c>
-      <c r="B29" s="3" t="s">
-        <v>177</v>
-      </c>
+        <v>175</v>
+      </c>
+      <c r="B29" s="3"/>
       <c r="D29" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E29" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="E29" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="G29" s="3" t="s">
         <v>112</v>
@@ -11917,27 +11907,25 @@
         <v>113</v>
       </c>
       <c r="I29" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="J29" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="J29" s="8" t="s">
+      <c r="K29" s="8" t="s">
         <v>174</v>
-      </c>
-      <c r="K29" s="8" t="s">
-        <v>175</v>
       </c>
     </row>
     <row r="30" spans="1:12" ht="15.75" customHeight="1">
       <c r="A30" s="3" t="s">
-        <v>178</v>
-      </c>
-      <c r="B30" s="3" t="s">
-        <v>179</v>
-      </c>
+        <v>176</v>
+      </c>
+      <c r="B30" s="3"/>
       <c r="D30" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="E30" s="3" t="s">
         <v>171</v>
-      </c>
-      <c r="E30" s="3" t="s">
-        <v>172</v>
       </c>
       <c r="G30" s="3" t="s">
         <v>112</v>
@@ -11946,16 +11934,16 @@
         <v>113</v>
       </c>
       <c r="I30" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="J30" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="J30" s="8" t="s">
+      <c r="K30" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="K30" s="8" t="s">
-        <v>175</v>
-      </c>
       <c r="L30" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1"/>
@@ -12939,7 +12927,7 @@
   <dimension ref="A1:E1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -13029,7 +13017,7 @@
     </row>
     <row r="6" spans="1:5" ht="149" customHeight="1">
       <c r="A6" s="4" t="s">
-        <v>582</v>
+        <v>579</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>84</v>
@@ -14036,7 +14024,7 @@
   <dimension ref="A1:C1000"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -14058,7 +14046,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="34">
+    <row r="2" spans="1:3" ht="51">
       <c r="A2" s="2" t="s">
         <v>144</v>
       </c>
@@ -14125,10 +14113,10 @@
         <v>159</v>
       </c>
       <c r="B8" s="22" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="15" customHeight="1">
@@ -15126,7 +15114,7 @@
   <dimension ref="A1:S988"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K7" sqref="K7"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -15155,78 +15143,78 @@
   <sheetData>
     <row r="1" spans="1:19" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="L1" s="12" t="s">
         <v>189</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="M1" s="12" t="s">
         <v>190</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="N1" s="9" t="s">
         <v>191</v>
       </c>
-      <c r="L1" s="12" t="s">
+      <c r="O1" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="M1" s="12" t="s">
+      <c r="P1" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="N1" s="9" t="s">
+      <c r="Q1" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="O1" s="9" t="s">
+      <c r="R1" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>196</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>197</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>198</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="2" spans="1:19" ht="67" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>200</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>201</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>202</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>203</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>204</v>
       </c>
       <c r="F2" s="2" t="s">
         <v>65</v>
@@ -15235,7 +15223,7 @@
         <v>66</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>65</v>
@@ -15244,13 +15232,13 @@
         <v>66</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>65</v>
@@ -15259,10 +15247,10 @@
         <v>66</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="Q2" s="2" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="R2" s="2" t="s">
         <v>65</v>
@@ -15276,111 +15264,111 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="H3" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="I3" s="2" t="s">
         <v>218</v>
       </c>
-      <c r="I3" s="2" t="s">
-        <v>221</v>
-      </c>
       <c r="J3" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>225</v>
+        <v>222</v>
       </c>
       <c r="L3" s="2" t="s">
+        <v>224</v>
+      </c>
+      <c r="M3" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="M3" s="2" t="s">
-        <v>230</v>
-      </c>
       <c r="N3" s="2" t="s">
-        <v>232</v>
+        <v>229</v>
       </c>
       <c r="O3" s="2" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="P3" s="2" t="s">
-        <v>236</v>
+        <v>233</v>
       </c>
       <c r="Q3" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
       <c r="R3" s="2" t="s">
-        <v>238</v>
+        <v>235</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="4" spans="1:19" hidden="1">
       <c r="A4" s="3" t="s">
-        <v>241</v>
+        <v>238</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="C4" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="D4" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>248</v>
-      </c>
       <c r="E4" s="3" t="s">
+        <v>246</v>
+      </c>
+      <c r="F4" s="3" t="s">
         <v>249</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>252</v>
-      </c>
       <c r="G4" s="3" t="s">
-        <v>254</v>
+        <v>251</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>260</v>
+        <v>257</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>262</v>
+        <v>259</v>
       </c>
       <c r="J4" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="L4" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="M4" s="5" t="s">
         <v>266</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>267</v>
       </c>
-      <c r="M4" s="5" t="s">
+      <c r="O4" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="P4" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="Q4" s="3" t="s">
-        <v>275</v>
-      </c>
       <c r="R4" s="3" t="s">
-        <v>277</v>
+        <v>274</v>
       </c>
       <c r="S4" s="3" t="s">
-        <v>279</v>
+        <v>276</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="30" customHeight="1">
@@ -15408,104 +15396,104 @@
     </row>
     <row r="6" spans="1:19">
       <c r="A6" s="3" t="s">
-        <v>322</v>
+        <v>319</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D6" s="11" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>326</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="K6" s="3" t="s">
         <v>329</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>328</v>
-      </c>
-      <c r="K6" s="3" t="s">
-        <v>332</v>
       </c>
       <c r="L6" s="3"/>
       <c r="M6" s="3"/>
       <c r="N6" s="3"/>
       <c r="O6" s="3"/>
       <c r="P6" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q6" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="R6" s="24" t="s">
         <v>337</v>
       </c>
-      <c r="R6" s="24" t="s">
-        <v>340</v>
-      </c>
       <c r="S6" s="20" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="7" spans="1:19">
       <c r="A7" s="3" t="s">
-        <v>343</v>
+        <v>340</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>323</v>
+        <v>320</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>324</v>
+        <v>321</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>331</v>
+        <v>328</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>330</v>
+        <v>327</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>329</v>
+        <v>326</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>328</v>
+        <v>325</v>
       </c>
       <c r="K7" s="3" t="s">
-        <v>344</v>
+        <v>341</v>
       </c>
       <c r="L7" s="3"/>
       <c r="M7" s="3"/>
       <c r="N7" s="3"/>
       <c r="O7" s="3"/>
       <c r="P7" s="5" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="Q7" s="20" t="s">
+        <v>334</v>
+      </c>
+      <c r="R7" s="24" t="s">
         <v>337</v>
       </c>
-      <c r="R7" s="24" t="s">
-        <v>340</v>
-      </c>
       <c r="S7" s="20" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
     </row>
     <row r="8" spans="1:19">
@@ -16521,54 +16509,54 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
+        <v>213</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>222</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>237</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>240</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>243</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="82.5" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>253</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>65</v>
@@ -16579,56 +16567,56 @@
     </row>
     <row r="3" spans="1:9" ht="51">
       <c r="A3" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:9" hidden="1">
       <c r="A4" s="3" t="s">
-        <v>287</v>
+        <v>284</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>288</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>290</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>291</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="E4" s="3" t="s">
+      <c r="F4" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="G4" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="F4" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>297</v>
-      </c>
       <c r="H4" s="3" t="s">
-        <v>299</v>
+        <v>296</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>301</v>
+        <v>298</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1">
@@ -16646,22 +16634,22 @@
     </row>
     <row r="6" spans="1:9" ht="64">
       <c r="A6" s="3" t="s">
-        <v>586</v>
+        <v>580</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>316</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="H6" s="10" t="s">
         <v>318</v>
       </c>
-      <c r="C6" s="7" t="s">
-        <v>319</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>320</v>
-      </c>
-      <c r="H6" s="10" t="s">
-        <v>321</v>
-      </c>
       <c r="I6" s="5" t="s">
-        <v>320</v>
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -17660,15 +17648,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:U987"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="43.6640625" customWidth="1"/>
     <col min="2" max="2" width="46.5" customWidth="1"/>
-    <col min="3" max="3" width="33.1640625" customWidth="1"/>
+    <col min="3" max="3" width="41.6640625" customWidth="1"/>
     <col min="4" max="4" width="28.5" customWidth="1"/>
     <col min="5" max="5" width="23.1640625" customWidth="1"/>
     <col min="6" max="6" width="19.1640625" customWidth="1"/>
@@ -17691,87 +17679,87 @@
   <sheetData>
     <row r="1" spans="1:21" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>583</v>
+        <v>606</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>584</v>
+        <v>607</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>585</v>
+        <v>608</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>235</v>
+        <v>232</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="I1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="J1" s="1" t="s">
-        <v>185</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>186</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>187</v>
-      </c>
       <c r="M1" s="1" t="s">
+        <v>211</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="N1" s="1" t="s">
-        <v>215</v>
-      </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="P1" s="1" t="s">
-        <v>220</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>224</v>
+        <v>221</v>
       </c>
       <c r="R1" s="1" t="s">
-        <v>226</v>
+        <v>223</v>
       </c>
       <c r="S1" s="1" t="s">
+        <v>225</v>
+      </c>
+      <c r="T1" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="T1" s="1" t="s">
+      <c r="U1" s="1" t="s">
         <v>231</v>
-      </c>
-      <c r="U1" s="1" t="s">
-        <v>234</v>
       </c>
     </row>
     <row r="2" spans="1:21" ht="145" customHeight="1">
       <c r="A2" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>201</v>
+        <v>198</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>200</v>
+        <v>197</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>239</v>
+        <v>236</v>
       </c>
       <c r="G2" s="2" t="s">
         <v>65</v>
@@ -17780,10 +17768,10 @@
         <v>66</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>244</v>
+        <v>241</v>
       </c>
       <c r="K2" s="2" t="s">
         <v>65</v>
@@ -17792,7 +17780,7 @@
         <v>66</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>247</v>
+        <v>244</v>
       </c>
       <c r="N2" s="2" t="s">
         <v>65</v>
@@ -17801,7 +17789,7 @@
         <v>66</v>
       </c>
       <c r="P2" s="2" t="s">
-        <v>251</v>
+        <v>248</v>
       </c>
       <c r="Q2" s="2" t="s">
         <v>65</v>
@@ -17810,13 +17798,13 @@
         <v>66</v>
       </c>
       <c r="S2" s="2" t="s">
+        <v>253</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>255</v>
+      </c>
+      <c r="U2" s="2" t="s">
         <v>256</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>258</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>259</v>
       </c>
     </row>
     <row r="3" spans="1:21" ht="123" customHeight="1">
@@ -17825,120 +17813,120 @@
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="G3" s="2" t="s">
-        <v>221</v>
+        <v>218</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>223</v>
+        <v>220</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="M3" s="2" t="s">
-        <v>280</v>
+        <v>277</v>
       </c>
       <c r="N3" s="2" t="s">
+        <v>279</v>
+      </c>
+      <c r="O3" s="2" t="s">
+        <v>277</v>
+      </c>
+      <c r="P3" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="Q3" s="2" t="s">
         <v>282</v>
       </c>
-      <c r="O3" s="2" t="s">
-        <v>280</v>
-      </c>
-      <c r="P3" s="2" t="s">
-        <v>284</v>
-      </c>
-      <c r="Q3" s="2" t="s">
+      <c r="R3" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="S3" s="2" t="s">
         <v>285</v>
       </c>
-      <c r="R3" s="2" t="s">
-        <v>286</v>
-      </c>
-      <c r="S3" s="2" t="s">
-        <v>288</v>
-      </c>
       <c r="T3" s="2" t="s">
-        <v>290</v>
+        <v>287</v>
       </c>
       <c r="U3" s="2" t="s">
-        <v>292</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:21" hidden="1">
       <c r="A4" s="3" t="s">
-        <v>296</v>
+        <v>293</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>298</v>
+        <v>295</v>
       </c>
       <c r="C4" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>284</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="G4" s="5" t="s">
         <v>300</v>
       </c>
-      <c r="D4" s="3" t="s">
-        <v>241</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>287</v>
-      </c>
-      <c r="F4" s="5" t="s">
+      <c r="H4" s="5" t="s">
+        <v>301</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="G4" s="5" t="s">
+      <c r="J4" s="3" t="s">
         <v>303</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="K4" s="3" t="s">
         <v>304</v>
       </c>
-      <c r="I4" s="3" t="s">
+      <c r="L4" s="3" t="s">
         <v>305</v>
       </c>
-      <c r="J4" s="3" t="s">
+      <c r="M4" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="K4" s="3" t="s">
+      <c r="N4" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="O4" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="M4" s="3" t="s">
+      <c r="P4" s="3" t="s">
         <v>309</v>
       </c>
-      <c r="N4" s="3" t="s">
+      <c r="Q4" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="O4" s="3" t="s">
+      <c r="R4" s="3" t="s">
         <v>311</v>
       </c>
-      <c r="P4" s="3" t="s">
+      <c r="S4" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="Q4" s="3" t="s">
+      <c r="T4" s="3" t="s">
         <v>313</v>
       </c>
-      <c r="R4" s="3" t="s">
+      <c r="U4" s="3" t="s">
         <v>314</v>
-      </c>
-      <c r="S4" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="T4" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="U4" s="3" t="s">
-        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:21" ht="30" customHeight="1">
@@ -17968,126 +17956,126 @@
     </row>
     <row r="6" spans="1:21">
       <c r="A6" s="3" t="s">
+        <v>322</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>323</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="F6" s="3" t="s">
         <v>325</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="G6" s="14" t="s">
         <v>326</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="H6" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="I6" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="J6" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="D6" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>586</v>
-      </c>
-      <c r="F6" s="3" t="s">
+      <c r="K6" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="G6" s="14" t="s">
-        <v>329</v>
-      </c>
-      <c r="H6" s="14" t="s">
-        <v>328</v>
-      </c>
-      <c r="I6" s="11" t="s">
-        <v>324</v>
-      </c>
-      <c r="J6" s="3" t="s">
+      <c r="L6" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="M6" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="K6" s="3" t="s">
+      <c r="N6" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="O6" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="M6" s="3" t="s">
+      <c r="P6" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="Q6" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="N6" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="O6" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="P6" s="3" t="s">
+      <c r="R6" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="S6" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="Q6" s="3" t="s">
+      <c r="T6" s="3" t="s">
         <v>336</v>
-      </c>
-      <c r="R6" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="S6" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="T6" s="3" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="7" spans="1:21">
       <c r="A7" s="3" t="s">
-        <v>341</v>
+        <v>338</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C7" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>340</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>580</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>325</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>326</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>325</v>
+      </c>
+      <c r="I7" s="11" t="s">
+        <v>321</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>327</v>
       </c>
-      <c r="D7" s="3" t="s">
-        <v>343</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>586</v>
-      </c>
-      <c r="F7" s="3" t="s">
+      <c r="K7" s="3" t="s">
         <v>328</v>
       </c>
-      <c r="G7" s="14" t="s">
-        <v>329</v>
-      </c>
-      <c r="H7" s="14" t="s">
-        <v>328</v>
-      </c>
-      <c r="I7" s="11" t="s">
-        <v>324</v>
-      </c>
-      <c r="J7" s="3" t="s">
+      <c r="L7" s="3" t="s">
+        <v>327</v>
+      </c>
+      <c r="M7" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="K7" s="3" t="s">
+      <c r="N7" s="3" t="s">
         <v>331</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="O7" s="3" t="s">
         <v>330</v>
       </c>
-      <c r="M7" s="3" t="s">
+      <c r="P7" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="Q7" s="3" t="s">
         <v>333</v>
       </c>
-      <c r="N7" s="3" t="s">
-        <v>334</v>
-      </c>
-      <c r="O7" s="3" t="s">
-        <v>333</v>
-      </c>
-      <c r="P7" s="3" t="s">
+      <c r="R7" s="3" t="s">
+        <v>332</v>
+      </c>
+      <c r="S7" s="5" t="s">
         <v>335</v>
       </c>
-      <c r="Q7" s="3" t="s">
+      <c r="T7" s="3" t="s">
         <v>336</v>
-      </c>
-      <c r="R7" s="3" t="s">
-        <v>335</v>
-      </c>
-      <c r="S7" s="5" t="s">
-        <v>338</v>
-      </c>
-      <c r="T7" s="3" t="s">
-        <v>339</v>
       </c>
     </row>
     <row r="8" spans="1:21" ht="15.75" customHeight="1"/>
@@ -19081,8 +19069,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I998"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N3" sqref="N3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -19098,54 +19086,54 @@
   <sheetData>
     <row r="1" spans="1:9" ht="30" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>610</v>
+        <v>342</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>588</v>
+        <v>613</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>590</v>
+        <v>614</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>346</v>
+        <v>343</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>347</v>
+        <v>344</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>348</v>
+        <v>345</v>
       </c>
     </row>
     <row r="2" spans="1:9" ht="67.5" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>247</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>250</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>253</v>
-      </c>
       <c r="C2" s="2" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>257</v>
+        <v>254</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>261</v>
+        <v>258</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G2" s="2" t="s">
-        <v>265</v>
+        <v>262</v>
       </c>
       <c r="H2" s="2" t="s">
         <v>65</v>
@@ -19156,56 +19144,56 @@
     </row>
     <row r="3" spans="1:9" ht="409.6">
       <c r="A3" s="2" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>274</v>
+        <v>271</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>276</v>
+        <v>273</v>
       </c>
       <c r="F3" s="2" t="s">
+        <v>275</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>278</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>281</v>
-      </c>
       <c r="H3" s="2" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
     </row>
     <row r="4" spans="1:9" hidden="1">
       <c r="A4" s="3" t="s">
+        <v>346</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>347</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>348</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>349</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="E4" s="3" t="s">
         <v>350</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>351</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>352</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="H4" s="3" t="s">
         <v>353</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="I4" s="3" t="s">
         <v>354</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>355</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>356</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>357</v>
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1">
@@ -19223,48 +19211,48 @@
     </row>
     <row r="6" spans="1:9" ht="48">
       <c r="A6" s="3" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>326</v>
+        <v>323</v>
       </c>
       <c r="C6" s="28" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D6" s="18"/>
       <c r="E6" s="18"/>
       <c r="F6" s="18"/>
       <c r="G6" s="27" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="H6" s="16" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="I6" s="5" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="80">
       <c r="A7" s="3" t="s">
-        <v>362</v>
+        <v>359</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>342</v>
+        <v>339</v>
       </c>
       <c r="C7" s="28" t="s">
-        <v>363</v>
+        <v>360</v>
       </c>
       <c r="D7" s="18"/>
       <c r="E7" s="18"/>
       <c r="F7" s="18"/>
       <c r="G7" s="29" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="H7" s="16" t="s">
-        <v>365</v>
+        <v>362</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>366</v>
+        <v>363</v>
       </c>
     </row>
     <row r="19" ht="15.75" customHeight="1"/>
@@ -20260,8 +20248,8 @@
   </sheetPr>
   <dimension ref="A1:J1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView topLeftCell="J1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="12.6640625" defaultRowHeight="15" customHeight="1"/>
@@ -20280,57 +20268,57 @@
   <sheetData>
     <row r="1" spans="1:10" ht="33" customHeight="1">
       <c r="A1" s="1" t="s">
-        <v>589</v>
+        <v>610</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>588</v>
+        <v>611</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>590</v>
+        <v>612</v>
       </c>
       <c r="D1" s="1" t="s">
         <v>4</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>229</v>
+        <v>226</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>233</v>
+        <v>230</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>594</v>
+        <v>584</v>
       </c>
       <c r="H1" s="26" t="s">
-        <v>595</v>
+        <v>585</v>
       </c>
       <c r="I1" s="26" t="s">
-        <v>596</v>
+        <v>586</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>545</v>
+        <v>542</v>
       </c>
     </row>
     <row r="2" spans="1:10" ht="80" customHeight="1">
       <c r="A2" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>536</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>252</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="B2" s="2" t="s">
-        <v>539</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>255</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>540</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>541</v>
+        <v>538</v>
       </c>
       <c r="F2" s="2" t="s">
-        <v>263</v>
+        <v>260</v>
       </c>
       <c r="G2" s="25" t="s">
-        <v>593</v>
+        <v>583</v>
       </c>
       <c r="H2" s="25" t="s">
         <v>65</v>
@@ -20339,7 +20327,7 @@
         <v>66</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>543</v>
+        <v>540</v>
       </c>
     </row>
     <row r="3" spans="1:10" ht="80" customHeight="1">
@@ -20347,55 +20335,55 @@
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>591</v>
+        <v>581</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>592</v>
+        <v>582</v>
       </c>
       <c r="F3" s="2"/>
       <c r="G3" s="25" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="H3" s="25" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="I3" s="25" t="s">
-        <v>281</v>
+        <v>278</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>546</v>
+        <v>543</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="44" hidden="1" customHeight="1">
       <c r="A4" s="3" t="s">
-        <v>414</v>
+        <v>411</v>
       </c>
       <c r="B4" s="3" t="s">
+        <v>544</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>545</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>546</v>
+      </c>
+      <c r="E4" s="3" t="s">
         <v>547</v>
       </c>
-      <c r="C4" s="3" t="s">
+      <c r="F4" s="3" t="s">
         <v>548</v>
       </c>
-      <c r="D4" s="3" t="s">
+      <c r="G4" s="3" t="s">
         <v>549</v>
       </c>
-      <c r="E4" s="3" t="s">
+      <c r="H4" s="15" t="s">
         <v>550</v>
       </c>
-      <c r="F4" s="3" t="s">
+      <c r="I4" s="15" t="s">
         <v>551</v>
       </c>
-      <c r="G4" s="3" t="s">
+      <c r="J4" s="3" t="s">
         <v>552</v>
-      </c>
-      <c r="H4" s="15" t="s">
-        <v>553</v>
-      </c>
-      <c r="I4" s="15" t="s">
-        <v>554</v>
-      </c>
-      <c r="J4" s="3" t="s">
-        <v>555</v>
       </c>
     </row>
     <row r="5" spans="1:10" ht="31" customHeight="1">
@@ -20414,45 +20402,45 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" s="3" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
       <c r="B6" s="3" t="s">
+        <v>553</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>554</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>555</v>
+      </c>
+      <c r="H6" s="13" t="s">
         <v>556</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="I6" s="13" t="s">
         <v>557</v>
       </c>
-      <c r="G6" s="3" t="s">
+      <c r="J6" s="3" t="s">
         <v>558</v>
-      </c>
-      <c r="H6" s="13" t="s">
-        <v>559</v>
-      </c>
-      <c r="I6" s="13" t="s">
-        <v>560</v>
-      </c>
-      <c r="J6" s="3" t="s">
-        <v>561</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="48">
       <c r="A7" s="3" t="s">
-        <v>562</v>
+        <v>559</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>563</v>
+        <v>560</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>611</v>
+        <v>600</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>558</v>
+        <v>555</v>
       </c>
       <c r="H7" s="13" t="s">
-        <v>559</v>
+        <v>556</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>560</v>
+        <v>557</v>
       </c>
     </row>
     <row r="8" spans="1:10">

</xml_diff>